<commit_message>
fix: Retirando mensagem com dd/mm/aaaa
</commit_message>
<xml_diff>
--- a/docs/modelo_importacao_xlsx.xlsx
+++ b/docs/modelo_importacao_xlsx.xlsx
@@ -24,7 +24,7 @@
   <si>
     <t xml:space="preserve">Orientações: 
 - Mantenha as colunas na mesma ordem, sem modificar o texto dos cabeçalhos
-- Preencha a data da fatura no formato MM/AAAA, ou DD/MM/AAAA usando números e a barra como separador
+- Preencha a data da fatura no formato MM/AAAA usando números e a barra como separador
 - Preencha os outros valores somente com números, usando , como separador decimal
 - Para faturas da modalidade tarifária Verde, preencha as colunas Fora ponta, deixando as colunas Consumo Ponta (kWh) e Demanda Ponta (kW) em branco</t>
   </si>
@@ -341,7 +341,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,7 +359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Ajusta valores default de tarifas de geração
</commit_message>
<xml_diff>
--- a/docs/modelo_importacao_xlsx.xlsx
+++ b/docs/modelo_importacao_xlsx.xlsx
@@ -24,7 +24,7 @@
   <si>
     <t xml:space="preserve">Orientações: 
 - Mantenha as colunas na mesma ordem, sem modificar o texto dos cabeçalhos
-- Preencha a data da fatura no formato MM/AAAA, ou DD/MM/AAAA usando números e a barra como separador
+- Preencha a data da fatura no formato MM/AAAA usando números e a barra como separador
 - Preencha os outros valores somente com números, usando , como separador decimal
 - Para faturas da modalidade tarifária Verde, preencha as colunas Fora ponta, deixando as colunas Consumo Ponta (kWh) e Demanda Ponta (kW) em branco</t>
   </si>
@@ -341,7 +341,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,7 +359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>